<commit_message>
Change to Doxygen for documentation
</commit_message>
<xml_diff>
--- a/src/lib/dictionary/dict.xlsx
+++ b/src/lib/dictionary/dict.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="23715" windowHeight="14355"/>
+    <workbookView xWindow="120" yWindow="135" windowWidth="23715" windowHeight="13740" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="DATA elements" sheetId="6" r:id="rId1"/>
@@ -27189,19 +27189,10 @@
     <t>Study Component Management SOP Class (Retired)</t>
   </si>
   <si>
-    <t>1.­2.840.10008.3.1.2.3.3</t>
-  </si>
-  <si>
     <t>Modality Performed Procedure Step SOP Class</t>
   </si>
   <si>
-    <t>1.­2.840.10008.3.1.2.3.4</t>
-  </si>
-  <si>
     <t>Modality Performed Procedure Step Retrieve SOP Class</t>
-  </si>
-  <si>
-    <t>1.­2.840.10008.3.1.2.3.5</t>
   </si>
   <si>
     <t>Modality Performed Procedure Step Notification SOP Class</t>
@@ -28540,6 +28531,18 @@
   </si>
   <si>
     <t>1.2.840.10008.5.1.4.39.1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.2.840.10008.3.1.2.3.3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.2.840.10008.3.1.2.3.4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.2.840.10008.3.1.2.3.5</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -28889,7 +28892,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H2963"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A1004" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
@@ -80378,7 +80381,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D299"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
+      <selection activeCell="A82" sqref="A82"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
@@ -81422,10 +81427,10 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" t="s">
+        <v>9504</v>
+      </c>
+      <c r="B79" t="s">
         <v>9057</v>
-      </c>
-      <c r="B79" t="s">
-        <v>9058</v>
       </c>
       <c r="C79" t="s">
         <v>8888</v>
@@ -81436,10 +81441,10 @@
     </row>
     <row r="80" spans="1:4">
       <c r="A80" t="s">
-        <v>9059</v>
+        <v>9505</v>
       </c>
       <c r="B80" t="s">
-        <v>9060</v>
+        <v>9058</v>
       </c>
       <c r="C80" t="s">
         <v>8888</v>
@@ -81450,10 +81455,10 @@
     </row>
     <row r="81" spans="1:4">
       <c r="A81" t="s">
-        <v>9061</v>
+        <v>9506</v>
       </c>
       <c r="B81" t="s">
-        <v>9062</v>
+        <v>9059</v>
       </c>
       <c r="C81" t="s">
         <v>8888</v>
@@ -81464,10 +81469,10 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82" t="s">
-        <v>9063</v>
+        <v>9060</v>
       </c>
       <c r="B82" t="s">
-        <v>9064</v>
+        <v>9061</v>
       </c>
       <c r="C82" t="s">
         <v>8888</v>
@@ -81478,10 +81483,10 @@
     </row>
     <row r="83" spans="1:4">
       <c r="A83" t="s">
-        <v>9065</v>
+        <v>9062</v>
       </c>
       <c r="B83" t="s">
-        <v>9066</v>
+        <v>9063</v>
       </c>
       <c r="C83" t="s">
         <v>9050</v>
@@ -81492,10 +81497,10 @@
     </row>
     <row r="84" spans="1:4">
       <c r="A84" t="s">
-        <v>9067</v>
+        <v>9064</v>
       </c>
       <c r="B84" t="s">
-        <v>9068</v>
+        <v>9065</v>
       </c>
       <c r="C84" t="s">
         <v>9050</v>
@@ -81506,10 +81511,10 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" t="s">
-        <v>9069</v>
+        <v>9066</v>
       </c>
       <c r="B85" t="s">
-        <v>9070</v>
+        <v>9067</v>
       </c>
       <c r="C85" t="s">
         <v>8888</v>
@@ -81520,13 +81525,13 @@
     </row>
     <row r="86" spans="1:4">
       <c r="A86" t="s">
-        <v>9071</v>
+        <v>9068</v>
       </c>
       <c r="B86" t="s">
-        <v>9072</v>
+        <v>9069</v>
       </c>
       <c r="C86" t="s">
-        <v>9073</v>
+        <v>9070</v>
       </c>
       <c r="D86" t="s">
         <v>8889</v>
@@ -81534,10 +81539,10 @@
     </row>
     <row r="87" spans="1:4">
       <c r="A87" t="s">
-        <v>9074</v>
+        <v>9071</v>
       </c>
       <c r="B87" t="s">
-        <v>9075</v>
+        <v>9072</v>
       </c>
       <c r="C87" t="s">
         <v>8888</v>
@@ -81548,10 +81553,10 @@
     </row>
     <row r="88" spans="1:4">
       <c r="A88" t="s">
-        <v>9076</v>
+        <v>9073</v>
       </c>
       <c r="B88" t="s">
-        <v>9077</v>
+        <v>9074</v>
       </c>
       <c r="C88" t="s">
         <v>8888</v>
@@ -81562,10 +81567,10 @@
     </row>
     <row r="89" spans="1:4">
       <c r="A89" t="s">
-        <v>9078</v>
+        <v>9075</v>
       </c>
       <c r="B89" t="s">
-        <v>9079</v>
+        <v>9076</v>
       </c>
       <c r="C89" t="s">
         <v>8888</v>
@@ -81576,10 +81581,10 @@
     </row>
     <row r="90" spans="1:4">
       <c r="A90" t="s">
-        <v>9080</v>
+        <v>9077</v>
       </c>
       <c r="B90" t="s">
-        <v>9081</v>
+        <v>9078</v>
       </c>
       <c r="C90" t="s">
         <v>8888</v>
@@ -81590,10 +81595,10 @@
     </row>
     <row r="91" spans="1:4">
       <c r="A91" t="s">
-        <v>9082</v>
+        <v>9079</v>
       </c>
       <c r="B91" t="s">
-        <v>9083</v>
+        <v>9080</v>
       </c>
       <c r="C91" t="s">
         <v>8888</v>
@@ -81604,10 +81609,10 @@
     </row>
     <row r="92" spans="1:4">
       <c r="A92" t="s">
-        <v>9084</v>
+        <v>9081</v>
       </c>
       <c r="B92" t="s">
-        <v>9085</v>
+        <v>9082</v>
       </c>
       <c r="C92" t="s">
         <v>9050</v>
@@ -81618,10 +81623,10 @@
     </row>
     <row r="93" spans="1:4">
       <c r="A93" t="s">
-        <v>9086</v>
+        <v>9083</v>
       </c>
       <c r="B93" t="s">
-        <v>9087</v>
+        <v>9084</v>
       </c>
       <c r="C93" t="s">
         <v>9050</v>
@@ -81632,10 +81637,10 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94" t="s">
-        <v>9088</v>
+        <v>9085</v>
       </c>
       <c r="B94" t="s">
-        <v>9089</v>
+        <v>9086</v>
       </c>
       <c r="C94" t="s">
         <v>8888</v>
@@ -81646,10 +81651,10 @@
     </row>
     <row r="95" spans="1:4">
       <c r="A95" t="s">
-        <v>9090</v>
+        <v>9087</v>
       </c>
       <c r="B95" t="s">
-        <v>9091</v>
+        <v>9088</v>
       </c>
       <c r="C95" t="s">
         <v>8888</v>
@@ -81660,10 +81665,10 @@
     </row>
     <row r="96" spans="1:4">
       <c r="A96" t="s">
-        <v>9092</v>
+        <v>9089</v>
       </c>
       <c r="B96" t="s">
-        <v>9093</v>
+        <v>9090</v>
       </c>
       <c r="C96" t="s">
         <v>8888</v>
@@ -81674,10 +81679,10 @@
     </row>
     <row r="97" spans="1:4">
       <c r="A97" t="s">
-        <v>9094</v>
+        <v>9091</v>
       </c>
       <c r="B97" t="s">
-        <v>9095</v>
+        <v>9092</v>
       </c>
       <c r="C97" t="s">
         <v>8888</v>
@@ -81688,13 +81693,13 @@
     </row>
     <row r="98" spans="1:4">
       <c r="A98" t="s">
-        <v>9096</v>
+        <v>9093</v>
       </c>
       <c r="B98" t="s">
-        <v>9097</v>
+        <v>9094</v>
       </c>
       <c r="C98" t="s">
-        <v>9098</v>
+        <v>9095</v>
       </c>
       <c r="D98" t="s">
         <v>8889</v>
@@ -81702,13 +81707,13 @@
     </row>
     <row r="99" spans="1:4">
       <c r="A99" t="s">
-        <v>9099</v>
+        <v>9096</v>
       </c>
       <c r="B99" t="s">
-        <v>9100</v>
+        <v>9097</v>
       </c>
       <c r="C99" t="s">
-        <v>9098</v>
+        <v>9095</v>
       </c>
       <c r="D99" t="s">
         <v>8889</v>
@@ -81716,10 +81721,10 @@
     </row>
     <row r="100" spans="1:4">
       <c r="A100" t="s">
-        <v>9101</v>
+        <v>9098</v>
       </c>
       <c r="B100" t="s">
-        <v>9102</v>
+        <v>9099</v>
       </c>
       <c r="C100" t="s">
         <v>9050</v>
@@ -81730,10 +81735,10 @@
     </row>
     <row r="101" spans="1:4">
       <c r="A101" t="s">
-        <v>9103</v>
+        <v>9100</v>
       </c>
       <c r="B101" t="s">
-        <v>9104</v>
+        <v>9101</v>
       </c>
       <c r="C101" t="s">
         <v>9050</v>
@@ -81744,10 +81749,10 @@
     </row>
     <row r="102" spans="1:4">
       <c r="A102" t="s">
-        <v>9105</v>
+        <v>9102</v>
       </c>
       <c r="B102" t="s">
-        <v>9106</v>
+        <v>9103</v>
       </c>
       <c r="C102" t="s">
         <v>8888</v>
@@ -81758,10 +81763,10 @@
     </row>
     <row r="103" spans="1:4">
       <c r="A103" t="s">
-        <v>9107</v>
+        <v>9104</v>
       </c>
       <c r="B103" t="s">
-        <v>9108</v>
+        <v>9105</v>
       </c>
       <c r="C103" t="s">
         <v>8888</v>
@@ -81772,10 +81777,10 @@
     </row>
     <row r="104" spans="1:4">
       <c r="A104" t="s">
-        <v>9109</v>
+        <v>9106</v>
       </c>
       <c r="B104" t="s">
-        <v>9110</v>
+        <v>9107</v>
       </c>
       <c r="C104" t="s">
         <v>8888</v>
@@ -81786,10 +81791,10 @@
     </row>
     <row r="105" spans="1:4">
       <c r="A105" t="s">
-        <v>9111</v>
+        <v>9108</v>
       </c>
       <c r="B105" t="s">
-        <v>9112</v>
+        <v>9109</v>
       </c>
       <c r="C105" t="s">
         <v>8888</v>
@@ -81800,13 +81805,13 @@
     </row>
     <row r="106" spans="1:4">
       <c r="A106" t="s">
-        <v>9113</v>
+        <v>9110</v>
       </c>
       <c r="B106" t="s">
-        <v>9114</v>
+        <v>9111</v>
       </c>
       <c r="C106" t="s">
-        <v>9115</v>
+        <v>9112</v>
       </c>
       <c r="D106" t="s">
         <v>8889</v>
@@ -81814,10 +81819,10 @@
     </row>
     <row r="107" spans="1:4">
       <c r="A107" t="s">
-        <v>9116</v>
+        <v>9113</v>
       </c>
       <c r="B107" t="s">
-        <v>9117</v>
+        <v>9114</v>
       </c>
       <c r="C107" t="s">
         <v>8888</v>
@@ -81828,10 +81833,10 @@
     </row>
     <row r="108" spans="1:4">
       <c r="A108" t="s">
-        <v>9118</v>
+        <v>9115</v>
       </c>
       <c r="B108" t="s">
-        <v>9119</v>
+        <v>9116</v>
       </c>
       <c r="C108" t="s">
         <v>8888</v>
@@ -81842,10 +81847,10 @@
     </row>
     <row r="109" spans="1:4">
       <c r="A109" t="s">
-        <v>9120</v>
+        <v>9117</v>
       </c>
       <c r="B109" t="s">
-        <v>9121</v>
+        <v>9118</v>
       </c>
       <c r="C109" t="s">
         <v>8888</v>
@@ -81856,10 +81861,10 @@
     </row>
     <row r="110" spans="1:4">
       <c r="A110" t="s">
-        <v>9122</v>
+        <v>9119</v>
       </c>
       <c r="B110" t="s">
-        <v>9123</v>
+        <v>9120</v>
       </c>
       <c r="C110" t="s">
         <v>8888</v>
@@ -81870,10 +81875,10 @@
     </row>
     <row r="111" spans="1:4">
       <c r="A111" t="s">
-        <v>9124</v>
+        <v>9121</v>
       </c>
       <c r="B111" t="s">
-        <v>9125</v>
+        <v>9122</v>
       </c>
       <c r="C111" t="s">
         <v>8888</v>
@@ -81884,10 +81889,10 @@
     </row>
     <row r="112" spans="1:4">
       <c r="A112" t="s">
-        <v>9126</v>
+        <v>9123</v>
       </c>
       <c r="B112" t="s">
-        <v>9127</v>
+        <v>9124</v>
       </c>
       <c r="C112" t="s">
         <v>9050</v>
@@ -81898,24 +81903,24 @@
     </row>
     <row r="113" spans="1:4">
       <c r="A113" t="s">
-        <v>9128</v>
+        <v>9125</v>
       </c>
       <c r="B113" t="s">
-        <v>9129</v>
+        <v>9126</v>
       </c>
       <c r="C113" t="s">
         <v>8888</v>
       </c>
       <c r="D113" t="s">
-        <v>9130</v>
+        <v>9127</v>
       </c>
     </row>
     <row r="114" spans="1:4">
       <c r="A114" t="s">
-        <v>9131</v>
+        <v>9128</v>
       </c>
       <c r="B114" t="s">
-        <v>9132</v>
+        <v>9129</v>
       </c>
       <c r="C114" t="s">
         <v>8888</v>
@@ -81926,10 +81931,10 @@
     </row>
     <row r="115" spans="1:4">
       <c r="A115" t="s">
-        <v>9133</v>
+        <v>9130</v>
       </c>
       <c r="B115" t="s">
-        <v>9475</v>
+        <v>9472</v>
       </c>
       <c r="C115" t="s">
         <v>8888</v>
@@ -81940,10 +81945,10 @@
     </row>
     <row r="116" spans="1:4">
       <c r="A116" t="s">
-        <v>9134</v>
+        <v>9131</v>
       </c>
       <c r="B116" t="s">
-        <v>9476</v>
+        <v>9473</v>
       </c>
       <c r="C116" t="s">
         <v>8888</v>
@@ -81954,10 +81959,10 @@
     </row>
     <row r="117" spans="1:4">
       <c r="A117" t="s">
-        <v>9135</v>
+        <v>9132</v>
       </c>
       <c r="B117" t="s">
-        <v>9477</v>
+        <v>9474</v>
       </c>
       <c r="C117" t="s">
         <v>8888</v>
@@ -81968,10 +81973,10 @@
     </row>
     <row r="118" spans="1:4">
       <c r="A118" t="s">
-        <v>9136</v>
+        <v>9133</v>
       </c>
       <c r="B118" t="s">
-        <v>9478</v>
+        <v>9475</v>
       </c>
       <c r="C118" t="s">
         <v>8888</v>
@@ -81982,10 +81987,10 @@
     </row>
     <row r="119" spans="1:4">
       <c r="A119" t="s">
-        <v>9137</v>
+        <v>9134</v>
       </c>
       <c r="B119" t="s">
-        <v>9479</v>
+        <v>9476</v>
       </c>
       <c r="C119" t="s">
         <v>8888</v>
@@ -81996,10 +82001,10 @@
     </row>
     <row r="120" spans="1:4">
       <c r="A120" t="s">
-        <v>9138</v>
+        <v>9135</v>
       </c>
       <c r="B120" t="s">
-        <v>9480</v>
+        <v>9477</v>
       </c>
       <c r="C120" t="s">
         <v>8888</v>
@@ -82010,10 +82015,10 @@
     </row>
     <row r="121" spans="1:4">
       <c r="A121" t="s">
-        <v>9139</v>
+        <v>9136</v>
       </c>
       <c r="B121" t="s">
-        <v>9140</v>
+        <v>9137</v>
       </c>
       <c r="C121" t="s">
         <v>8888</v>
@@ -82024,10 +82029,10 @@
     </row>
     <row r="122" spans="1:4">
       <c r="A122" t="s">
-        <v>9141</v>
+        <v>9138</v>
       </c>
       <c r="B122" t="s">
-        <v>9142</v>
+        <v>9139</v>
       </c>
       <c r="C122" t="s">
         <v>8888</v>
@@ -82038,10 +82043,10 @@
     </row>
     <row r="123" spans="1:4">
       <c r="A123" t="s">
-        <v>9143</v>
+        <v>9140</v>
       </c>
       <c r="B123" t="s">
-        <v>9144</v>
+        <v>9141</v>
       </c>
       <c r="C123" t="s">
         <v>8888</v>
@@ -82052,10 +82057,10 @@
     </row>
     <row r="124" spans="1:4">
       <c r="A124" t="s">
-        <v>9145</v>
+        <v>9142</v>
       </c>
       <c r="B124" t="s">
-        <v>9146</v>
+        <v>9143</v>
       </c>
       <c r="C124" t="s">
         <v>8888</v>
@@ -82066,10 +82071,10 @@
     </row>
     <row r="125" spans="1:4">
       <c r="A125" t="s">
-        <v>9147</v>
+        <v>9144</v>
       </c>
       <c r="B125" t="s">
-        <v>9148</v>
+        <v>9145</v>
       </c>
       <c r="C125" t="s">
         <v>8888</v>
@@ -82080,10 +82085,10 @@
     </row>
     <row r="126" spans="1:4">
       <c r="A126" t="s">
-        <v>9149</v>
+        <v>9146</v>
       </c>
       <c r="B126" t="s">
-        <v>9150</v>
+        <v>9147</v>
       </c>
       <c r="C126" t="s">
         <v>8888</v>
@@ -82094,10 +82099,10 @@
     </row>
     <row r="127" spans="1:4">
       <c r="A127" t="s">
-        <v>9151</v>
+        <v>9148</v>
       </c>
       <c r="B127" t="s">
-        <v>9152</v>
+        <v>9149</v>
       </c>
       <c r="C127" t="s">
         <v>8888</v>
@@ -82108,10 +82113,10 @@
     </row>
     <row r="128" spans="1:4">
       <c r="A128" t="s">
-        <v>9153</v>
+        <v>9150</v>
       </c>
       <c r="B128" t="s">
-        <v>9154</v>
+        <v>9151</v>
       </c>
       <c r="C128" t="s">
         <v>8888</v>
@@ -82122,10 +82127,10 @@
     </row>
     <row r="129" spans="1:4">
       <c r="A129" t="s">
-        <v>9155</v>
+        <v>9152</v>
       </c>
       <c r="B129" t="s">
-        <v>9156</v>
+        <v>9153</v>
       </c>
       <c r="C129" t="s">
         <v>8888</v>
@@ -82136,10 +82141,10 @@
     </row>
     <row r="130" spans="1:4">
       <c r="A130" t="s">
-        <v>9157</v>
+        <v>9154</v>
       </c>
       <c r="B130" t="s">
-        <v>9158</v>
+        <v>9155</v>
       </c>
       <c r="C130" t="s">
         <v>8888</v>
@@ -82150,10 +82155,10 @@
     </row>
     <row r="131" spans="1:4">
       <c r="A131" t="s">
-        <v>9159</v>
+        <v>9156</v>
       </c>
       <c r="B131" t="s">
-        <v>9160</v>
+        <v>9157</v>
       </c>
       <c r="C131" t="s">
         <v>8888</v>
@@ -82164,10 +82169,10 @@
     </row>
     <row r="132" spans="1:4">
       <c r="A132" t="s">
-        <v>9161</v>
+        <v>9158</v>
       </c>
       <c r="B132" t="s">
-        <v>9162</v>
+        <v>9159</v>
       </c>
       <c r="C132" t="s">
         <v>8888</v>
@@ -82178,10 +82183,10 @@
     </row>
     <row r="133" spans="1:4">
       <c r="A133" t="s">
-        <v>9163</v>
+        <v>9160</v>
       </c>
       <c r="B133" t="s">
-        <v>9164</v>
+        <v>9161</v>
       </c>
       <c r="C133" t="s">
         <v>8888</v>
@@ -82192,10 +82197,10 @@
     </row>
     <row r="134" spans="1:4">
       <c r="A134" t="s">
-        <v>9165</v>
+        <v>9162</v>
       </c>
       <c r="B134" t="s">
-        <v>9166</v>
+        <v>9163</v>
       </c>
       <c r="C134" t="s">
         <v>8888</v>
@@ -82206,10 +82211,10 @@
     </row>
     <row r="135" spans="1:4">
       <c r="A135" t="s">
-        <v>9167</v>
+        <v>9164</v>
       </c>
       <c r="B135" t="s">
-        <v>9168</v>
+        <v>9165</v>
       </c>
       <c r="C135" t="s">
         <v>8888</v>
@@ -82220,10 +82225,10 @@
     </row>
     <row r="136" spans="1:4">
       <c r="A136" t="s">
-        <v>9169</v>
+        <v>9166</v>
       </c>
       <c r="B136" t="s">
-        <v>9170</v>
+        <v>9167</v>
       </c>
       <c r="C136" t="s">
         <v>8888</v>
@@ -82234,10 +82239,10 @@
     </row>
     <row r="137" spans="1:4">
       <c r="A137" t="s">
-        <v>9171</v>
+        <v>9168</v>
       </c>
       <c r="B137" t="s">
-        <v>9172</v>
+        <v>9169</v>
       </c>
       <c r="C137" t="s">
         <v>8888</v>
@@ -82248,10 +82253,10 @@
     </row>
     <row r="138" spans="1:4">
       <c r="A138" t="s">
-        <v>9173</v>
+        <v>9170</v>
       </c>
       <c r="B138" t="s">
-        <v>9174</v>
+        <v>9171</v>
       </c>
       <c r="C138" t="s">
         <v>8888</v>
@@ -82262,10 +82267,10 @@
     </row>
     <row r="139" spans="1:4">
       <c r="A139" t="s">
-        <v>9175</v>
+        <v>9172</v>
       </c>
       <c r="B139" t="s">
-        <v>9176</v>
+        <v>9173</v>
       </c>
       <c r="C139" t="s">
         <v>8888</v>
@@ -82276,10 +82281,10 @@
     </row>
     <row r="140" spans="1:4">
       <c r="A140" t="s">
-        <v>9177</v>
+        <v>9174</v>
       </c>
       <c r="B140" t="s">
-        <v>9178</v>
+        <v>9175</v>
       </c>
       <c r="C140" t="s">
         <v>8888</v>
@@ -82290,10 +82295,10 @@
     </row>
     <row r="141" spans="1:4">
       <c r="A141" t="s">
-        <v>9179</v>
+        <v>9176</v>
       </c>
       <c r="B141" t="s">
-        <v>9180</v>
+        <v>9177</v>
       </c>
       <c r="C141" t="s">
         <v>8888</v>
@@ -82304,10 +82309,10 @@
     </row>
     <row r="142" spans="1:4">
       <c r="A142" t="s">
-        <v>9181</v>
+        <v>9178</v>
       </c>
       <c r="B142" t="s">
-        <v>9182</v>
+        <v>9179</v>
       </c>
       <c r="C142" t="s">
         <v>8888</v>
@@ -82318,10 +82323,10 @@
     </row>
     <row r="143" spans="1:4">
       <c r="A143" t="s">
-        <v>9183</v>
+        <v>9180</v>
       </c>
       <c r="B143" t="s">
-        <v>9184</v>
+        <v>9181</v>
       </c>
       <c r="C143" t="s">
         <v>8888</v>
@@ -82332,10 +82337,10 @@
     </row>
     <row r="144" spans="1:4">
       <c r="A144" t="s">
-        <v>9185</v>
+        <v>9182</v>
       </c>
       <c r="B144" t="s">
-        <v>9186</v>
+        <v>9183</v>
       </c>
       <c r="C144" t="s">
         <v>8888</v>
@@ -82346,10 +82351,10 @@
     </row>
     <row r="145" spans="1:4">
       <c r="A145" t="s">
-        <v>9187</v>
+        <v>9184</v>
       </c>
       <c r="B145" t="s">
-        <v>9188</v>
+        <v>9185</v>
       </c>
       <c r="C145" t="s">
         <v>8888</v>
@@ -82360,10 +82365,10 @@
     </row>
     <row r="146" spans="1:4">
       <c r="A146" t="s">
-        <v>9189</v>
+        <v>9186</v>
       </c>
       <c r="B146" t="s">
-        <v>9190</v>
+        <v>9187</v>
       </c>
       <c r="C146" t="s">
         <v>8888</v>
@@ -82374,10 +82379,10 @@
     </row>
     <row r="147" spans="1:4">
       <c r="A147" t="s">
-        <v>9191</v>
+        <v>9188</v>
       </c>
       <c r="B147" t="s">
-        <v>9192</v>
+        <v>9189</v>
       </c>
       <c r="C147" t="s">
         <v>8888</v>
@@ -82388,10 +82393,10 @@
     </row>
     <row r="148" spans="1:4">
       <c r="A148" t="s">
-        <v>9193</v>
+        <v>9190</v>
       </c>
       <c r="B148" t="s">
-        <v>9194</v>
+        <v>9191</v>
       </c>
       <c r="C148" t="s">
         <v>8888</v>
@@ -82402,10 +82407,10 @@
     </row>
     <row r="149" spans="1:4">
       <c r="A149" t="s">
-        <v>9195</v>
+        <v>9192</v>
       </c>
       <c r="B149" t="s">
-        <v>9196</v>
+        <v>9193</v>
       </c>
       <c r="C149" t="s">
         <v>8888</v>
@@ -82416,10 +82421,10 @@
     </row>
     <row r="150" spans="1:4">
       <c r="A150" t="s">
-        <v>9197</v>
+        <v>9194</v>
       </c>
       <c r="B150" t="s">
-        <v>9198</v>
+        <v>9195</v>
       </c>
       <c r="C150" t="s">
         <v>8888</v>
@@ -82430,10 +82435,10 @@
     </row>
     <row r="151" spans="1:4">
       <c r="A151" t="s">
-        <v>9199</v>
+        <v>9196</v>
       </c>
       <c r="B151" t="s">
-        <v>9200</v>
+        <v>9197</v>
       </c>
       <c r="C151" t="s">
         <v>8888</v>
@@ -82444,10 +82449,10 @@
     </row>
     <row r="152" spans="1:4">
       <c r="A152" t="s">
-        <v>9201</v>
+        <v>9198</v>
       </c>
       <c r="B152" t="s">
-        <v>9202</v>
+        <v>9199</v>
       </c>
       <c r="C152" t="s">
         <v>8888</v>
@@ -82458,10 +82463,10 @@
     </row>
     <row r="153" spans="1:4">
       <c r="A153" t="s">
-        <v>9203</v>
+        <v>9200</v>
       </c>
       <c r="B153" t="s">
-        <v>9204</v>
+        <v>9201</v>
       </c>
       <c r="C153" t="s">
         <v>8888</v>
@@ -82472,10 +82477,10 @@
     </row>
     <row r="154" spans="1:4">
       <c r="A154" t="s">
-        <v>9205</v>
+        <v>9202</v>
       </c>
       <c r="B154" t="s">
-        <v>9206</v>
+        <v>9203</v>
       </c>
       <c r="C154" t="s">
         <v>8888</v>
@@ -82486,10 +82491,10 @@
     </row>
     <row r="155" spans="1:4">
       <c r="A155" t="s">
-        <v>9207</v>
+        <v>9204</v>
       </c>
       <c r="B155" t="s">
-        <v>9208</v>
+        <v>9205</v>
       </c>
       <c r="C155" t="s">
         <v>8888</v>
@@ -82500,10 +82505,10 @@
     </row>
     <row r="156" spans="1:4">
       <c r="A156" t="s">
-        <v>9209</v>
+        <v>9206</v>
       </c>
       <c r="B156" t="s">
-        <v>9210</v>
+        <v>9207</v>
       </c>
       <c r="C156" t="s">
         <v>8888</v>
@@ -82514,10 +82519,10 @@
     </row>
     <row r="157" spans="1:4">
       <c r="A157" t="s">
-        <v>9211</v>
+        <v>9208</v>
       </c>
       <c r="B157" t="s">
-        <v>9212</v>
+        <v>9209</v>
       </c>
       <c r="C157" t="s">
         <v>8888</v>
@@ -82528,10 +82533,10 @@
     </row>
     <row r="158" spans="1:4">
       <c r="A158" t="s">
-        <v>9213</v>
+        <v>9210</v>
       </c>
       <c r="B158" t="s">
-        <v>9214</v>
+        <v>9211</v>
       </c>
       <c r="C158" t="s">
         <v>8888</v>
@@ -82542,10 +82547,10 @@
     </row>
     <row r="159" spans="1:4">
       <c r="A159" t="s">
-        <v>9215</v>
+        <v>9212</v>
       </c>
       <c r="B159" t="s">
-        <v>9216</v>
+        <v>9213</v>
       </c>
       <c r="C159" t="s">
         <v>8888</v>
@@ -82556,10 +82561,10 @@
     </row>
     <row r="160" spans="1:4">
       <c r="A160" t="s">
-        <v>9217</v>
+        <v>9214</v>
       </c>
       <c r="B160" t="s">
-        <v>9218</v>
+        <v>9215</v>
       </c>
       <c r="C160" t="s">
         <v>8888</v>
@@ -82570,10 +82575,10 @@
     </row>
     <row r="161" spans="1:4">
       <c r="A161" t="s">
-        <v>9219</v>
+        <v>9216</v>
       </c>
       <c r="B161" t="s">
-        <v>9220</v>
+        <v>9217</v>
       </c>
       <c r="C161" t="s">
         <v>8888</v>
@@ -82584,10 +82589,10 @@
     </row>
     <row r="162" spans="1:4">
       <c r="A162" t="s">
-        <v>9221</v>
+        <v>9218</v>
       </c>
       <c r="B162" t="s">
-        <v>9222</v>
+        <v>9219</v>
       </c>
       <c r="C162" t="s">
         <v>8888</v>
@@ -82598,10 +82603,10 @@
     </row>
     <row r="163" spans="1:4">
       <c r="A163" t="s">
-        <v>9223</v>
+        <v>9220</v>
       </c>
       <c r="B163" t="s">
-        <v>9224</v>
+        <v>9221</v>
       </c>
       <c r="C163" t="s">
         <v>8888</v>
@@ -82612,10 +82617,10 @@
     </row>
     <row r="164" spans="1:4">
       <c r="A164" t="s">
-        <v>9225</v>
+        <v>9222</v>
       </c>
       <c r="B164" t="s">
-        <v>9226</v>
+        <v>9223</v>
       </c>
       <c r="C164" t="s">
         <v>8888</v>
@@ -82626,10 +82631,10 @@
     </row>
     <row r="165" spans="1:4">
       <c r="A165" t="s">
-        <v>9227</v>
+        <v>9224</v>
       </c>
       <c r="B165" t="s">
-        <v>9228</v>
+        <v>9225</v>
       </c>
       <c r="C165" t="s">
         <v>8888</v>
@@ -82640,10 +82645,10 @@
     </row>
     <row r="166" spans="1:4">
       <c r="A166" t="s">
-        <v>9229</v>
+        <v>9226</v>
       </c>
       <c r="B166" t="s">
-        <v>9230</v>
+        <v>9227</v>
       </c>
       <c r="C166" t="s">
         <v>8888</v>
@@ -82654,10 +82659,10 @@
     </row>
     <row r="167" spans="1:4">
       <c r="A167" t="s">
-        <v>9231</v>
+        <v>9228</v>
       </c>
       <c r="B167" t="s">
-        <v>9232</v>
+        <v>9229</v>
       </c>
       <c r="C167" t="s">
         <v>8888</v>
@@ -82668,10 +82673,10 @@
     </row>
     <row r="168" spans="1:4">
       <c r="A168" t="s">
-        <v>9233</v>
+        <v>9230</v>
       </c>
       <c r="B168" t="s">
-        <v>9234</v>
+        <v>9231</v>
       </c>
       <c r="C168" t="s">
         <v>8888</v>
@@ -82682,10 +82687,10 @@
     </row>
     <row r="169" spans="1:4">
       <c r="A169" t="s">
-        <v>9235</v>
+        <v>9232</v>
       </c>
       <c r="B169" t="s">
-        <v>9236</v>
+        <v>9233</v>
       </c>
       <c r="C169" t="s">
         <v>8888</v>
@@ -82696,10 +82701,10 @@
     </row>
     <row r="170" spans="1:4">
       <c r="A170" t="s">
-        <v>9237</v>
+        <v>9234</v>
       </c>
       <c r="B170" t="s">
-        <v>9238</v>
+        <v>9235</v>
       </c>
       <c r="C170" t="s">
         <v>8888</v>
@@ -82710,10 +82715,10 @@
     </row>
     <row r="171" spans="1:4">
       <c r="A171" t="s">
-        <v>9239</v>
+        <v>9236</v>
       </c>
       <c r="B171" t="s">
-        <v>9240</v>
+        <v>9237</v>
       </c>
       <c r="C171" t="s">
         <v>8888</v>
@@ -82724,10 +82729,10 @@
     </row>
     <row r="172" spans="1:4">
       <c r="A172" t="s">
-        <v>9241</v>
+        <v>9238</v>
       </c>
       <c r="B172" t="s">
-        <v>9503</v>
+        <v>9500</v>
       </c>
       <c r="C172" t="s">
         <v>8888</v>
@@ -82738,26 +82743,26 @@
     </row>
     <row r="173" spans="1:4">
       <c r="A173" t="s">
-        <v>9242</v>
+        <v>9239</v>
       </c>
       <c r="B173" t="s">
-        <v>9243</v>
+        <v>9240</v>
       </c>
     </row>
     <row r="174" spans="1:4">
       <c r="A174" t="s">
-        <v>9244</v>
+        <v>9241</v>
       </c>
       <c r="B174" t="s">
-        <v>9481</v>
+        <v>9478</v>
       </c>
     </row>
     <row r="175" spans="1:4">
       <c r="A175" t="s">
-        <v>9245</v>
+        <v>9242</v>
       </c>
       <c r="B175" t="s">
-        <v>9246</v>
+        <v>9243</v>
       </c>
       <c r="C175" t="s">
         <v>8888</v>
@@ -82768,10 +82773,10 @@
     </row>
     <row r="176" spans="1:4">
       <c r="A176" t="s">
-        <v>9247</v>
+        <v>9244</v>
       </c>
       <c r="B176" t="s">
-        <v>9248</v>
+        <v>9245</v>
       </c>
       <c r="C176" t="s">
         <v>8888</v>
@@ -82782,10 +82787,10 @@
     </row>
     <row r="177" spans="1:4">
       <c r="A177" t="s">
-        <v>9249</v>
+        <v>9246</v>
       </c>
       <c r="B177" t="s">
-        <v>9250</v>
+        <v>9247</v>
       </c>
       <c r="C177" t="s">
         <v>8888</v>
@@ -82796,10 +82801,10 @@
     </row>
     <row r="178" spans="1:4">
       <c r="A178" t="s">
-        <v>9251</v>
+        <v>9248</v>
       </c>
       <c r="B178" t="s">
-        <v>9252</v>
+        <v>9249</v>
       </c>
       <c r="C178" t="s">
         <v>8888</v>
@@ -82810,10 +82815,10 @@
     </row>
     <row r="179" spans="1:4">
       <c r="A179" t="s">
-        <v>9253</v>
+        <v>9250</v>
       </c>
       <c r="B179" t="s">
-        <v>9254</v>
+        <v>9251</v>
       </c>
       <c r="C179" t="s">
         <v>8888</v>
@@ -82824,10 +82829,10 @@
     </row>
     <row r="180" spans="1:4">
       <c r="A180" t="s">
-        <v>9255</v>
+        <v>9252</v>
       </c>
       <c r="B180" t="s">
-        <v>9256</v>
+        <v>9253</v>
       </c>
       <c r="C180" t="s">
         <v>8888</v>
@@ -82838,10 +82843,10 @@
     </row>
     <row r="181" spans="1:4">
       <c r="A181" t="s">
-        <v>9257</v>
+        <v>9254</v>
       </c>
       <c r="B181" t="s">
-        <v>9258</v>
+        <v>9255</v>
       </c>
       <c r="C181" t="s">
         <v>8888</v>
@@ -82852,10 +82857,10 @@
     </row>
     <row r="182" spans="1:4">
       <c r="A182" t="s">
-        <v>9259</v>
+        <v>9256</v>
       </c>
       <c r="B182" t="s">
-        <v>9260</v>
+        <v>9257</v>
       </c>
       <c r="C182" t="s">
         <v>8888</v>
@@ -82866,10 +82871,10 @@
     </row>
     <row r="183" spans="1:4">
       <c r="A183" t="s">
-        <v>9261</v>
+        <v>9258</v>
       </c>
       <c r="B183" t="s">
-        <v>9262</v>
+        <v>9259</v>
       </c>
       <c r="C183" t="s">
         <v>8888</v>
@@ -82880,10 +82885,10 @@
     </row>
     <row r="184" spans="1:4">
       <c r="A184" t="s">
-        <v>9263</v>
+        <v>9260</v>
       </c>
       <c r="B184" t="s">
-        <v>9264</v>
+        <v>9261</v>
       </c>
       <c r="C184" t="s">
         <v>8888</v>
@@ -82894,10 +82899,10 @@
     </row>
     <row r="185" spans="1:4">
       <c r="A185" t="s">
-        <v>9265</v>
+        <v>9262</v>
       </c>
       <c r="B185" t="s">
-        <v>9266</v>
+        <v>9263</v>
       </c>
       <c r="C185" t="s">
         <v>8888</v>
@@ -82908,10 +82913,10 @@
     </row>
     <row r="186" spans="1:4">
       <c r="A186" t="s">
-        <v>9267</v>
+        <v>9264</v>
       </c>
       <c r="B186" t="s">
-        <v>9268</v>
+        <v>9265</v>
       </c>
       <c r="C186" t="s">
         <v>8888</v>
@@ -82922,10 +82927,10 @@
     </row>
     <row r="187" spans="1:4">
       <c r="A187" t="s">
-        <v>9269</v>
+        <v>9266</v>
       </c>
       <c r="B187" t="s">
-        <v>9270</v>
+        <v>9267</v>
       </c>
       <c r="C187" t="s">
         <v>8888</v>
@@ -82936,10 +82941,10 @@
     </row>
     <row r="188" spans="1:4">
       <c r="A188" t="s">
-        <v>9271</v>
+        <v>9268</v>
       </c>
       <c r="B188" t="s">
-        <v>9272</v>
+        <v>9269</v>
       </c>
       <c r="C188" t="s">
         <v>8888</v>
@@ -82950,10 +82955,10 @@
     </row>
     <row r="189" spans="1:4">
       <c r="A189" t="s">
-        <v>9273</v>
+        <v>9270</v>
       </c>
       <c r="B189" t="s">
-        <v>9274</v>
+        <v>9271</v>
       </c>
       <c r="C189" t="s">
         <v>8888</v>
@@ -82964,10 +82969,10 @@
     </row>
     <row r="190" spans="1:4">
       <c r="A190" t="s">
-        <v>9275</v>
+        <v>9272</v>
       </c>
       <c r="B190" t="s">
-        <v>9276</v>
+        <v>9273</v>
       </c>
       <c r="C190" t="s">
         <v>8888</v>
@@ -82978,10 +82983,10 @@
     </row>
     <row r="191" spans="1:4">
       <c r="A191" t="s">
-        <v>9277</v>
+        <v>9274</v>
       </c>
       <c r="B191" t="s">
-        <v>9278</v>
+        <v>9275</v>
       </c>
       <c r="C191" t="s">
         <v>8888</v>
@@ -82992,10 +82997,10 @@
     </row>
     <row r="192" spans="1:4">
       <c r="A192" t="s">
-        <v>9279</v>
+        <v>9276</v>
       </c>
       <c r="B192" t="s">
-        <v>9280</v>
+        <v>9277</v>
       </c>
       <c r="C192" t="s">
         <v>8888</v>
@@ -83006,10 +83011,10 @@
     </row>
     <row r="193" spans="1:4">
       <c r="A193" t="s">
-        <v>9281</v>
+        <v>9278</v>
       </c>
       <c r="B193" t="s">
-        <v>9482</v>
+        <v>9479</v>
       </c>
       <c r="C193" t="s">
         <v>8888</v>
@@ -83020,10 +83025,10 @@
     </row>
     <row r="194" spans="1:4">
       <c r="A194" t="s">
-        <v>9282</v>
+        <v>9279</v>
       </c>
       <c r="B194" t="s">
-        <v>9483</v>
+        <v>9480</v>
       </c>
       <c r="C194" t="s">
         <v>8888</v>
@@ -83034,10 +83039,10 @@
     </row>
     <row r="195" spans="1:4">
       <c r="A195" t="s">
-        <v>9283</v>
+        <v>9280</v>
       </c>
       <c r="B195" t="s">
-        <v>9484</v>
+        <v>9481</v>
       </c>
       <c r="C195" t="s">
         <v>8888</v>
@@ -83048,10 +83053,10 @@
     </row>
     <row r="196" spans="1:4">
       <c r="A196" t="s">
-        <v>9284</v>
+        <v>9281</v>
       </c>
       <c r="B196" t="s">
-        <v>9485</v>
+        <v>9482</v>
       </c>
       <c r="C196" t="s">
         <v>8888</v>
@@ -83062,10 +83067,10 @@
     </row>
     <row r="197" spans="1:4">
       <c r="A197" t="s">
-        <v>9285</v>
+        <v>9282</v>
       </c>
       <c r="B197" t="s">
-        <v>9286</v>
+        <v>9283</v>
       </c>
       <c r="C197" t="s">
         <v>8888</v>
@@ -83076,10 +83081,10 @@
     </row>
     <row r="198" spans="1:4">
       <c r="A198" t="s">
-        <v>9287</v>
+        <v>9284</v>
       </c>
       <c r="B198" t="s">
-        <v>9288</v>
+        <v>9285</v>
       </c>
       <c r="C198" t="s">
         <v>8888</v>
@@ -83090,10 +83095,10 @@
     </row>
     <row r="199" spans="1:4">
       <c r="A199" t="s">
-        <v>9289</v>
+        <v>9286</v>
       </c>
       <c r="B199" t="s">
-        <v>9290</v>
+        <v>9287</v>
       </c>
       <c r="C199" t="s">
         <v>8888</v>
@@ -83104,10 +83109,10 @@
     </row>
     <row r="200" spans="1:4">
       <c r="A200" t="s">
-        <v>9291</v>
+        <v>9288</v>
       </c>
       <c r="B200" t="s">
-        <v>9292</v>
+        <v>9289</v>
       </c>
       <c r="C200" t="s">
         <v>8888</v>
@@ -83118,10 +83123,10 @@
     </row>
     <row r="201" spans="1:4">
       <c r="A201" t="s">
-        <v>9293</v>
+        <v>9290</v>
       </c>
       <c r="B201" t="s">
-        <v>9294</v>
+        <v>9291</v>
       </c>
       <c r="C201" t="s">
         <v>8888</v>
@@ -83132,10 +83137,10 @@
     </row>
     <row r="202" spans="1:4">
       <c r="A202" t="s">
-        <v>9295</v>
+        <v>9292</v>
       </c>
       <c r="B202" t="s">
-        <v>9296</v>
+        <v>9293</v>
       </c>
       <c r="C202" t="s">
         <v>8888</v>
@@ -83146,10 +83151,10 @@
     </row>
     <row r="203" spans="1:4">
       <c r="A203" t="s">
-        <v>9297</v>
+        <v>9294</v>
       </c>
       <c r="B203" t="s">
-        <v>9298</v>
+        <v>9295</v>
       </c>
       <c r="C203" t="s">
         <v>8888</v>
@@ -83160,10 +83165,10 @@
     </row>
     <row r="204" spans="1:4">
       <c r="A204" t="s">
-        <v>9299</v>
+        <v>9296</v>
       </c>
       <c r="B204" t="s">
-        <v>9300</v>
+        <v>9297</v>
       </c>
       <c r="C204" t="s">
         <v>8888</v>
@@ -83174,10 +83179,10 @@
     </row>
     <row r="205" spans="1:4">
       <c r="A205" t="s">
-        <v>9301</v>
+        <v>9298</v>
       </c>
       <c r="B205" t="s">
-        <v>9302</v>
+        <v>9299</v>
       </c>
       <c r="C205" t="s">
         <v>8888</v>
@@ -83188,10 +83193,10 @@
     </row>
     <row r="206" spans="1:4">
       <c r="A206" t="s">
-        <v>9303</v>
+        <v>9300</v>
       </c>
       <c r="B206" t="s">
-        <v>9304</v>
+        <v>9301</v>
       </c>
       <c r="C206" t="s">
         <v>8888</v>
@@ -83202,10 +83207,10 @@
     </row>
     <row r="207" spans="1:4">
       <c r="A207" t="s">
-        <v>9305</v>
+        <v>9302</v>
       </c>
       <c r="B207" t="s">
-        <v>9306</v>
+        <v>9303</v>
       </c>
       <c r="C207" t="s">
         <v>8888</v>
@@ -83216,10 +83221,10 @@
     </row>
     <row r="208" spans="1:4">
       <c r="A208" t="s">
-        <v>9307</v>
+        <v>9304</v>
       </c>
       <c r="B208" t="s">
-        <v>9308</v>
+        <v>9305</v>
       </c>
       <c r="C208" t="s">
         <v>8888</v>
@@ -83230,10 +83235,10 @@
     </row>
     <row r="209" spans="1:4">
       <c r="A209" t="s">
-        <v>9309</v>
+        <v>9306</v>
       </c>
       <c r="B209" t="s">
-        <v>9310</v>
+        <v>9307</v>
       </c>
       <c r="C209" t="s">
         <v>8888</v>
@@ -83244,10 +83249,10 @@
     </row>
     <row r="210" spans="1:4">
       <c r="A210" t="s">
-        <v>9311</v>
+        <v>9308</v>
       </c>
       <c r="B210" t="s">
-        <v>9312</v>
+        <v>9309</v>
       </c>
       <c r="C210" t="s">
         <v>8888</v>
@@ -83258,10 +83263,10 @@
     </row>
     <row r="211" spans="1:4">
       <c r="A211" t="s">
-        <v>9313</v>
+        <v>9310</v>
       </c>
       <c r="B211" t="s">
-        <v>9314</v>
+        <v>9311</v>
       </c>
       <c r="C211" t="s">
         <v>8888</v>
@@ -83272,10 +83277,10 @@
     </row>
     <row r="212" spans="1:4">
       <c r="A212" t="s">
-        <v>9315</v>
+        <v>9312</v>
       </c>
       <c r="B212" t="s">
-        <v>9316</v>
+        <v>9313</v>
       </c>
       <c r="C212" t="s">
         <v>8888</v>
@@ -83286,10 +83291,10 @@
     </row>
     <row r="213" spans="1:4">
       <c r="A213" t="s">
-        <v>9317</v>
+        <v>9314</v>
       </c>
       <c r="B213" t="s">
-        <v>9318</v>
+        <v>9315</v>
       </c>
       <c r="C213" t="s">
         <v>8888</v>
@@ -83300,10 +83305,10 @@
     </row>
     <row r="214" spans="1:4">
       <c r="A214" t="s">
-        <v>9319</v>
+        <v>9316</v>
       </c>
       <c r="B214" t="s">
-        <v>9320</v>
+        <v>9317</v>
       </c>
       <c r="C214" t="s">
         <v>8888</v>
@@ -83314,10 +83319,10 @@
     </row>
     <row r="215" spans="1:4">
       <c r="A215" t="s">
-        <v>9321</v>
+        <v>9318</v>
       </c>
       <c r="B215" t="s">
-        <v>9322</v>
+        <v>9319</v>
       </c>
       <c r="C215" t="s">
         <v>8888</v>
@@ -83328,10 +83333,10 @@
     </row>
     <row r="216" spans="1:4">
       <c r="A216" t="s">
-        <v>9323</v>
+        <v>9320</v>
       </c>
       <c r="B216" t="s">
-        <v>9324</v>
+        <v>9321</v>
       </c>
       <c r="C216" t="s">
         <v>8888</v>
@@ -83342,10 +83347,10 @@
     </row>
     <row r="217" spans="1:4">
       <c r="A217" t="s">
-        <v>9325</v>
+        <v>9322</v>
       </c>
       <c r="B217" t="s">
-        <v>9326</v>
+        <v>9323</v>
       </c>
       <c r="C217" t="s">
         <v>8888</v>
@@ -83356,10 +83361,10 @@
     </row>
     <row r="218" spans="1:4">
       <c r="A218" t="s">
-        <v>9327</v>
+        <v>9324</v>
       </c>
       <c r="B218" t="s">
-        <v>9328</v>
+        <v>9325</v>
       </c>
       <c r="C218" t="s">
         <v>8888</v>
@@ -83370,10 +83375,10 @@
     </row>
     <row r="219" spans="1:4">
       <c r="A219" t="s">
-        <v>9329</v>
+        <v>9326</v>
       </c>
       <c r="B219" t="s">
-        <v>9330</v>
+        <v>9327</v>
       </c>
       <c r="C219" t="s">
         <v>8888</v>
@@ -83384,10 +83389,10 @@
     </row>
     <row r="220" spans="1:4">
       <c r="A220" t="s">
-        <v>9331</v>
+        <v>9328</v>
       </c>
       <c r="B220" t="s">
-        <v>9332</v>
+        <v>9329</v>
       </c>
       <c r="C220" t="s">
         <v>8888</v>
@@ -83398,10 +83403,10 @@
     </row>
     <row r="221" spans="1:4">
       <c r="A221" t="s">
-        <v>9333</v>
+        <v>9330</v>
       </c>
       <c r="B221" t="s">
-        <v>9486</v>
+        <v>9483</v>
       </c>
       <c r="C221" t="s">
         <v>8888</v>
@@ -83412,10 +83417,10 @@
     </row>
     <row r="222" spans="1:4">
       <c r="A222" t="s">
-        <v>9334</v>
+        <v>9331</v>
       </c>
       <c r="B222" t="s">
-        <v>9487</v>
+        <v>9484</v>
       </c>
       <c r="C222" t="s">
         <v>8888</v>
@@ -83426,10 +83431,10 @@
     </row>
     <row r="223" spans="1:4">
       <c r="A223" t="s">
-        <v>9335</v>
+        <v>9332</v>
       </c>
       <c r="B223" t="s">
-        <v>9488</v>
+        <v>9485</v>
       </c>
       <c r="C223" t="s">
         <v>8888</v>
@@ -83440,10 +83445,10 @@
     </row>
     <row r="224" spans="1:4">
       <c r="A224" t="s">
-        <v>9336</v>
+        <v>9333</v>
       </c>
       <c r="B224" t="s">
-        <v>9489</v>
+        <v>9486</v>
       </c>
       <c r="C224" t="s">
         <v>8888</v>
@@ -83454,10 +83459,10 @@
     </row>
     <row r="225" spans="1:4">
       <c r="A225" t="s">
-        <v>9337</v>
+        <v>9334</v>
       </c>
       <c r="B225" t="s">
-        <v>9490</v>
+        <v>9487</v>
       </c>
       <c r="C225" t="s">
         <v>8888</v>
@@ -83468,10 +83473,10 @@
     </row>
     <row r="226" spans="1:4">
       <c r="A226" t="s">
-        <v>9338</v>
+        <v>9335</v>
       </c>
       <c r="B226" t="s">
-        <v>9491</v>
+        <v>9488</v>
       </c>
       <c r="C226" t="s">
         <v>8888</v>
@@ -83482,10 +83487,10 @@
     </row>
     <row r="227" spans="1:4">
       <c r="A227" t="s">
-        <v>9339</v>
+        <v>9336</v>
       </c>
       <c r="B227" t="s">
-        <v>9340</v>
+        <v>9337</v>
       </c>
       <c r="C227" t="s">
         <v>8888</v>
@@ -83496,10 +83501,10 @@
     </row>
     <row r="228" spans="1:4">
       <c r="A228" t="s">
-        <v>9341</v>
+        <v>9338</v>
       </c>
       <c r="B228" t="s">
-        <v>9342</v>
+        <v>9339</v>
       </c>
       <c r="C228" t="s">
         <v>8888</v>
@@ -83510,10 +83515,10 @@
     </row>
     <row r="229" spans="1:4">
       <c r="A229" t="s">
-        <v>9343</v>
+        <v>9340</v>
       </c>
       <c r="B229" t="s">
-        <v>9344</v>
+        <v>9341</v>
       </c>
       <c r="C229" t="s">
         <v>8888</v>
@@ -83524,10 +83529,10 @@
     </row>
     <row r="230" spans="1:4">
       <c r="A230" t="s">
-        <v>9345</v>
+        <v>9342</v>
       </c>
       <c r="B230" t="s">
-        <v>9346</v>
+        <v>9343</v>
       </c>
       <c r="C230" t="s">
         <v>8888</v>
@@ -83538,10 +83543,10 @@
     </row>
     <row r="231" spans="1:4">
       <c r="A231" t="s">
-        <v>9347</v>
+        <v>9344</v>
       </c>
       <c r="B231" t="s">
-        <v>9348</v>
+        <v>9345</v>
       </c>
       <c r="C231" t="s">
         <v>8888</v>
@@ -83552,10 +83557,10 @@
     </row>
     <row r="232" spans="1:4">
       <c r="A232" t="s">
-        <v>9349</v>
+        <v>9346</v>
       </c>
       <c r="B232" t="s">
-        <v>9350</v>
+        <v>9347</v>
       </c>
       <c r="C232" t="s">
         <v>8888</v>
@@ -83566,10 +83571,10 @@
     </row>
     <row r="233" spans="1:4">
       <c r="A233" t="s">
-        <v>9351</v>
+        <v>9348</v>
       </c>
       <c r="B233" t="s">
-        <v>9492</v>
+        <v>9489</v>
       </c>
       <c r="C233" t="s">
         <v>8888</v>
@@ -83580,10 +83585,10 @@
     </row>
     <row r="234" spans="1:4">
       <c r="A234" t="s">
-        <v>9352</v>
+        <v>9349</v>
       </c>
       <c r="B234" t="s">
-        <v>9493</v>
+        <v>9490</v>
       </c>
       <c r="C234" t="s">
         <v>8888</v>
@@ -83594,10 +83599,10 @@
     </row>
     <row r="235" spans="1:4">
       <c r="A235" t="s">
-        <v>9353</v>
+        <v>9350</v>
       </c>
       <c r="B235" t="s">
-        <v>9354</v>
+        <v>9351</v>
       </c>
       <c r="C235" t="s">
         <v>8888</v>
@@ -83608,10 +83613,10 @@
     </row>
     <row r="236" spans="1:4">
       <c r="A236" t="s">
-        <v>9355</v>
+        <v>9352</v>
       </c>
       <c r="B236" t="s">
-        <v>9356</v>
+        <v>9353</v>
       </c>
       <c r="C236" t="s">
         <v>8888</v>
@@ -83622,10 +83627,10 @@
     </row>
     <row r="237" spans="1:4">
       <c r="A237" t="s">
-        <v>9357</v>
+        <v>9354</v>
       </c>
       <c r="B237" t="s">
-        <v>9358</v>
+        <v>9355</v>
       </c>
       <c r="C237" t="s">
         <v>9050</v>
@@ -83636,10 +83641,10 @@
     </row>
     <row r="238" spans="1:4">
       <c r="A238" t="s">
-        <v>9359</v>
+        <v>9356</v>
       </c>
       <c r="B238" t="s">
-        <v>9360</v>
+        <v>9357</v>
       </c>
       <c r="C238" t="s">
         <v>8888</v>
@@ -83650,10 +83655,10 @@
     </row>
     <row r="239" spans="1:4">
       <c r="A239" t="s">
-        <v>9361</v>
+        <v>9358</v>
       </c>
       <c r="B239" t="s">
-        <v>9362</v>
+        <v>9359</v>
       </c>
       <c r="C239" t="s">
         <v>8888</v>
@@ -83664,10 +83669,10 @@
     </row>
     <row r="240" spans="1:4">
       <c r="A240" t="s">
-        <v>9363</v>
+        <v>9360</v>
       </c>
       <c r="B240" t="s">
-        <v>9364</v>
+        <v>9361</v>
       </c>
       <c r="C240" t="s">
         <v>8888</v>
@@ -83678,10 +83683,10 @@
     </row>
     <row r="241" spans="1:4">
       <c r="A241" t="s">
-        <v>9365</v>
+        <v>9362</v>
       </c>
       <c r="B241" t="s">
-        <v>9366</v>
+        <v>9363</v>
       </c>
       <c r="C241" t="s">
         <v>8888</v>
@@ -83692,13 +83697,13 @@
     </row>
     <row r="242" spans="1:4">
       <c r="A242" t="s">
-        <v>9367</v>
+        <v>9364</v>
       </c>
       <c r="B242" t="s">
-        <v>9504</v>
+        <v>9501</v>
       </c>
       <c r="C242" t="s">
-        <v>9073</v>
+        <v>9070</v>
       </c>
       <c r="D242" t="s">
         <v>8889</v>
@@ -83706,10 +83711,10 @@
     </row>
     <row r="243" spans="1:4">
       <c r="A243" t="s">
-        <v>9368</v>
+        <v>9365</v>
       </c>
       <c r="B243" t="s">
-        <v>9494</v>
+        <v>9491</v>
       </c>
       <c r="C243" t="s">
         <v>8888</v>
@@ -83720,10 +83725,10 @@
     </row>
     <row r="244" spans="1:4">
       <c r="A244" t="s">
-        <v>9369</v>
+        <v>9366</v>
       </c>
       <c r="B244" t="s">
-        <v>9495</v>
+        <v>9492</v>
       </c>
       <c r="C244" t="s">
         <v>8888</v>
@@ -83734,10 +83739,10 @@
     </row>
     <row r="245" spans="1:4">
       <c r="A245" t="s">
-        <v>9370</v>
+        <v>9367</v>
       </c>
       <c r="B245" t="s">
-        <v>9496</v>
+        <v>9493</v>
       </c>
       <c r="C245" t="s">
         <v>8888</v>
@@ -83748,10 +83753,10 @@
     </row>
     <row r="246" spans="1:4">
       <c r="A246" t="s">
-        <v>9371</v>
+        <v>9368</v>
       </c>
       <c r="B246" t="s">
-        <v>9497</v>
+        <v>9494</v>
       </c>
       <c r="C246" t="s">
         <v>8888</v>
@@ -83762,10 +83767,10 @@
     </row>
     <row r="247" spans="1:4">
       <c r="A247" t="s">
-        <v>9372</v>
+        <v>9369</v>
       </c>
       <c r="B247" t="s">
-        <v>9373</v>
+        <v>9370</v>
       </c>
       <c r="C247" t="s">
         <v>9009</v>
@@ -83776,10 +83781,10 @@
     </row>
     <row r="248" spans="1:4">
       <c r="A248" t="s">
-        <v>9374</v>
+        <v>9371</v>
       </c>
       <c r="B248" t="s">
-        <v>9375</v>
+        <v>9372</v>
       </c>
       <c r="C248" t="s">
         <v>8888</v>
@@ -83790,10 +83795,10 @@
     </row>
     <row r="249" spans="1:4">
       <c r="A249" t="s">
-        <v>9376</v>
+        <v>9373</v>
       </c>
       <c r="B249" t="s">
-        <v>9377</v>
+        <v>9374</v>
       </c>
       <c r="C249" t="s">
         <v>8888</v>
@@ -83804,10 +83809,10 @@
     </row>
     <row r="250" spans="1:4">
       <c r="A250" t="s">
-        <v>9378</v>
+        <v>9375</v>
       </c>
       <c r="B250" t="s">
-        <v>9379</v>
+        <v>9376</v>
       </c>
       <c r="C250" t="s">
         <v>8888</v>
@@ -83818,10 +83823,10 @@
     </row>
     <row r="251" spans="1:4">
       <c r="A251" t="s">
-        <v>9380</v>
+        <v>9377</v>
       </c>
       <c r="B251" t="s">
-        <v>9381</v>
+        <v>9378</v>
       </c>
       <c r="C251" t="s">
         <v>8888</v>
@@ -83832,10 +83837,10 @@
     </row>
     <row r="252" spans="1:4">
       <c r="A252" t="s">
-        <v>9382</v>
+        <v>9379</v>
       </c>
       <c r="B252" t="s">
-        <v>9498</v>
+        <v>9495</v>
       </c>
       <c r="C252" t="s">
         <v>8888</v>
@@ -83846,10 +83851,10 @@
     </row>
     <row r="253" spans="1:4">
       <c r="A253" t="s">
-        <v>9383</v>
+        <v>9380</v>
       </c>
       <c r="B253" t="s">
-        <v>9499</v>
+        <v>9496</v>
       </c>
       <c r="C253" t="s">
         <v>8888</v>
@@ -83860,10 +83865,10 @@
     </row>
     <row r="254" spans="1:4">
       <c r="A254" t="s">
-        <v>9384</v>
+        <v>9381</v>
       </c>
       <c r="B254" t="s">
-        <v>9385</v>
+        <v>9382</v>
       </c>
       <c r="C254" t="s">
         <v>8888</v>
@@ -83874,13 +83879,13 @@
     </row>
     <row r="255" spans="1:4">
       <c r="A255" t="s">
-        <v>9506</v>
+        <v>9503</v>
       </c>
       <c r="B255" t="s">
-        <v>9505</v>
+        <v>9502</v>
       </c>
       <c r="C255" t="s">
-        <v>9386</v>
+        <v>9383</v>
       </c>
       <c r="D255" t="s">
         <v>8889</v>
@@ -83888,13 +83893,13 @@
     </row>
     <row r="256" spans="1:4">
       <c r="A256" t="s">
-        <v>9387</v>
+        <v>9384</v>
       </c>
       <c r="B256" t="s">
-        <v>9500</v>
+        <v>9497</v>
       </c>
       <c r="C256" t="s">
-        <v>9388</v>
+        <v>9385</v>
       </c>
       <c r="D256" t="s">
         <v>8889</v>
@@ -83902,13 +83907,13 @@
     </row>
     <row r="257" spans="1:4">
       <c r="A257" t="s">
-        <v>9389</v>
+        <v>9386</v>
       </c>
       <c r="B257" t="s">
-        <v>9501</v>
+        <v>9498</v>
       </c>
       <c r="C257" t="s">
-        <v>9388</v>
+        <v>9385</v>
       </c>
       <c r="D257" t="s">
         <v>8889</v>
@@ -83916,13 +83921,13 @@
     </row>
     <row r="258" spans="1:4">
       <c r="A258" t="s">
-        <v>9390</v>
+        <v>9387</v>
       </c>
       <c r="B258" t="s">
-        <v>9502</v>
+        <v>9499</v>
       </c>
       <c r="C258" t="s">
-        <v>9388</v>
+        <v>9385</v>
       </c>
       <c r="D258" t="s">
         <v>8889</v>
@@ -83930,10 +83935,10 @@
     </row>
     <row r="259" spans="1:4">
       <c r="A259" t="s">
-        <v>9391</v>
+        <v>9388</v>
       </c>
       <c r="B259" t="s">
-        <v>9392</v>
+        <v>9389</v>
       </c>
       <c r="C259" t="s">
         <v>8888</v>
@@ -83944,10 +83949,10 @@
     </row>
     <row r="260" spans="1:4">
       <c r="A260" t="s">
-        <v>9393</v>
+        <v>9390</v>
       </c>
       <c r="B260" t="s">
-        <v>9394</v>
+        <v>9391</v>
       </c>
       <c r="C260" t="s">
         <v>8888</v>
@@ -83958,548 +83963,548 @@
     </row>
     <row r="261" spans="1:4">
       <c r="A261" t="s">
+        <v>9392</v>
+      </c>
+      <c r="B261" t="s">
+        <v>9393</v>
+      </c>
+      <c r="C261" t="s">
+        <v>9394</v>
+      </c>
+      <c r="D261" t="s">
         <v>9395</v>
-      </c>
-      <c r="B261" t="s">
-        <v>9396</v>
-      </c>
-      <c r="C261" t="s">
-        <v>9397</v>
-      </c>
-      <c r="D261" t="s">
-        <v>9398</v>
       </c>
     </row>
     <row r="262" spans="1:4">
       <c r="A262" t="s">
-        <v>9399</v>
+        <v>9396</v>
       </c>
       <c r="B262" t="s">
-        <v>9400</v>
+        <v>9397</v>
       </c>
       <c r="C262" t="s">
-        <v>9397</v>
+        <v>9394</v>
       </c>
       <c r="D262" t="s">
-        <v>9398</v>
+        <v>9395</v>
       </c>
     </row>
     <row r="263" spans="1:4">
       <c r="A263" t="s">
-        <v>9401</v>
+        <v>9398</v>
       </c>
       <c r="B263" t="s">
-        <v>9402</v>
+        <v>9399</v>
       </c>
       <c r="C263" t="s">
-        <v>9397</v>
+        <v>9394</v>
       </c>
       <c r="D263" t="s">
-        <v>9398</v>
+        <v>9395</v>
       </c>
     </row>
     <row r="264" spans="1:4">
       <c r="A264" t="s">
-        <v>9403</v>
+        <v>9400</v>
       </c>
       <c r="B264" t="s">
-        <v>9404</v>
+        <v>9401</v>
       </c>
       <c r="C264" t="s">
-        <v>9397</v>
+        <v>9394</v>
       </c>
       <c r="D264" t="s">
-        <v>9398</v>
+        <v>9395</v>
       </c>
     </row>
     <row r="265" spans="1:4">
       <c r="A265" t="s">
-        <v>9405</v>
+        <v>9402</v>
       </c>
       <c r="B265" t="s">
-        <v>9406</v>
+        <v>9403</v>
       </c>
       <c r="C265" t="s">
-        <v>9397</v>
+        <v>9394</v>
       </c>
       <c r="D265" t="s">
-        <v>9398</v>
+        <v>9395</v>
       </c>
     </row>
     <row r="266" spans="1:4">
       <c r="A266" t="s">
-        <v>9407</v>
+        <v>9404</v>
       </c>
       <c r="B266" t="s">
-        <v>9408</v>
+        <v>9405</v>
       </c>
       <c r="C266" t="s">
-        <v>9397</v>
+        <v>9394</v>
       </c>
       <c r="D266" t="s">
-        <v>9398</v>
+        <v>9395</v>
       </c>
     </row>
     <row r="267" spans="1:4">
       <c r="A267" t="s">
-        <v>9409</v>
+        <v>9406</v>
       </c>
       <c r="B267" t="s">
-        <v>9410</v>
+        <v>9407</v>
       </c>
       <c r="C267" t="s">
-        <v>9397</v>
+        <v>9394</v>
       </c>
       <c r="D267" t="s">
-        <v>9398</v>
+        <v>9395</v>
       </c>
     </row>
     <row r="268" spans="1:4">
       <c r="A268" t="s">
-        <v>9411</v>
+        <v>9408</v>
       </c>
       <c r="B268" t="s">
-        <v>9412</v>
+        <v>9409</v>
       </c>
       <c r="C268" t="s">
-        <v>9397</v>
+        <v>9394</v>
       </c>
       <c r="D268" t="s">
-        <v>9398</v>
+        <v>9395</v>
       </c>
     </row>
     <row r="269" spans="1:4">
       <c r="A269" t="s">
-        <v>9413</v>
+        <v>9410</v>
       </c>
       <c r="B269" t="s">
-        <v>9414</v>
+        <v>9411</v>
       </c>
       <c r="C269" t="s">
-        <v>9397</v>
+        <v>9394</v>
       </c>
       <c r="D269" t="s">
-        <v>9398</v>
+        <v>9395</v>
       </c>
     </row>
     <row r="270" spans="1:4">
       <c r="A270" t="s">
-        <v>9415</v>
+        <v>9412</v>
       </c>
       <c r="B270" t="s">
-        <v>9416</v>
+        <v>9413</v>
       </c>
       <c r="C270" t="s">
-        <v>9397</v>
+        <v>9394</v>
       </c>
       <c r="D270" t="s">
-        <v>9398</v>
+        <v>9395</v>
       </c>
     </row>
     <row r="271" spans="1:4">
       <c r="A271" t="s">
-        <v>9417</v>
+        <v>9414</v>
       </c>
       <c r="B271" t="s">
-        <v>9418</v>
+        <v>9415</v>
       </c>
       <c r="C271" t="s">
-        <v>9397</v>
+        <v>9394</v>
       </c>
       <c r="D271" t="s">
-        <v>9398</v>
+        <v>9395</v>
       </c>
     </row>
     <row r="272" spans="1:4">
       <c r="A272" t="s">
-        <v>9419</v>
+        <v>9416</v>
       </c>
       <c r="B272" t="s">
-        <v>9420</v>
+        <v>9417</v>
       </c>
       <c r="C272" t="s">
-        <v>9397</v>
+        <v>9394</v>
       </c>
       <c r="D272" t="s">
-        <v>9398</v>
+        <v>9395</v>
       </c>
     </row>
     <row r="273" spans="1:4">
       <c r="A273" t="s">
-        <v>9421</v>
+        <v>9418</v>
       </c>
       <c r="B273" t="s">
-        <v>9422</v>
+        <v>9419</v>
       </c>
       <c r="C273" t="s">
-        <v>9397</v>
+        <v>9394</v>
       </c>
       <c r="D273" t="s">
-        <v>9398</v>
+        <v>9395</v>
       </c>
     </row>
     <row r="274" spans="1:4">
       <c r="A274" t="s">
-        <v>9423</v>
+        <v>9420</v>
       </c>
       <c r="B274" t="s">
-        <v>9424</v>
+        <v>9421</v>
       </c>
       <c r="C274" t="s">
-        <v>9397</v>
+        <v>9394</v>
       </c>
       <c r="D274" t="s">
-        <v>9398</v>
+        <v>9395</v>
       </c>
     </row>
     <row r="275" spans="1:4">
       <c r="A275" t="s">
-        <v>9425</v>
+        <v>9422</v>
       </c>
       <c r="B275" t="s">
-        <v>9426</v>
+        <v>9423</v>
       </c>
       <c r="C275" t="s">
-        <v>9397</v>
+        <v>9394</v>
       </c>
       <c r="D275" t="s">
-        <v>9398</v>
+        <v>9395</v>
       </c>
     </row>
     <row r="276" spans="1:4">
       <c r="A276" t="s">
-        <v>9427</v>
+        <v>9424</v>
       </c>
       <c r="B276" t="s">
-        <v>9428</v>
+        <v>9425</v>
       </c>
       <c r="C276" t="s">
-        <v>9397</v>
+        <v>9394</v>
       </c>
       <c r="D276" t="s">
-        <v>9398</v>
+        <v>9395</v>
       </c>
     </row>
     <row r="277" spans="1:4">
       <c r="A277" t="s">
-        <v>9429</v>
+        <v>9426</v>
       </c>
       <c r="B277" t="s">
-        <v>9430</v>
+        <v>9427</v>
       </c>
       <c r="C277" t="s">
-        <v>9397</v>
+        <v>9394</v>
       </c>
       <c r="D277" t="s">
-        <v>9398</v>
+        <v>9395</v>
       </c>
     </row>
     <row r="278" spans="1:4">
       <c r="A278" t="s">
-        <v>9431</v>
+        <v>9428</v>
       </c>
       <c r="B278" t="s">
-        <v>9432</v>
+        <v>9429</v>
       </c>
       <c r="C278" t="s">
-        <v>9397</v>
+        <v>9394</v>
       </c>
       <c r="D278" t="s">
-        <v>9398</v>
+        <v>9395</v>
       </c>
     </row>
     <row r="279" spans="1:4">
       <c r="A279" t="s">
-        <v>9433</v>
+        <v>9430</v>
       </c>
       <c r="B279" t="s">
-        <v>9434</v>
+        <v>9431</v>
       </c>
       <c r="C279" t="s">
-        <v>9397</v>
+        <v>9394</v>
       </c>
       <c r="D279" t="s">
-        <v>9398</v>
+        <v>9395</v>
       </c>
     </row>
     <row r="280" spans="1:4">
       <c r="A280" t="s">
-        <v>9435</v>
+        <v>9432</v>
       </c>
       <c r="B280" t="s">
-        <v>9436</v>
+        <v>9433</v>
       </c>
       <c r="C280" t="s">
-        <v>9397</v>
+        <v>9394</v>
       </c>
       <c r="D280" t="s">
-        <v>9398</v>
+        <v>9395</v>
       </c>
     </row>
     <row r="281" spans="1:4">
       <c r="A281" t="s">
-        <v>9437</v>
+        <v>9434</v>
       </c>
       <c r="B281" t="s">
-        <v>9438</v>
+        <v>9435</v>
       </c>
       <c r="C281" t="s">
-        <v>9397</v>
+        <v>9394</v>
       </c>
       <c r="D281" t="s">
-        <v>9398</v>
+        <v>9395</v>
       </c>
     </row>
     <row r="282" spans="1:4">
       <c r="A282" t="s">
-        <v>9439</v>
+        <v>9436</v>
       </c>
       <c r="B282" t="s">
-        <v>9440</v>
+        <v>9437</v>
       </c>
       <c r="C282" t="s">
-        <v>9397</v>
+        <v>9394</v>
       </c>
       <c r="D282" t="s">
-        <v>9398</v>
+        <v>9395</v>
       </c>
     </row>
     <row r="283" spans="1:4">
       <c r="A283" t="s">
-        <v>9441</v>
+        <v>9438</v>
       </c>
       <c r="B283" t="s">
-        <v>9442</v>
+        <v>9439</v>
       </c>
       <c r="C283" t="s">
-        <v>9397</v>
+        <v>9394</v>
       </c>
       <c r="D283" t="s">
-        <v>9398</v>
+        <v>9395</v>
       </c>
     </row>
     <row r="284" spans="1:4">
       <c r="A284" t="s">
-        <v>9443</v>
+        <v>9440</v>
       </c>
       <c r="B284" t="s">
-        <v>9444</v>
+        <v>9441</v>
       </c>
       <c r="C284" t="s">
-        <v>9397</v>
+        <v>9394</v>
       </c>
       <c r="D284" t="s">
-        <v>9398</v>
+        <v>9395</v>
       </c>
     </row>
     <row r="285" spans="1:4">
       <c r="A285" t="s">
-        <v>9445</v>
+        <v>9442</v>
       </c>
       <c r="B285" t="s">
-        <v>9446</v>
+        <v>9443</v>
       </c>
       <c r="C285" t="s">
-        <v>9397</v>
+        <v>9394</v>
       </c>
       <c r="D285" t="s">
-        <v>9398</v>
+        <v>9395</v>
       </c>
     </row>
     <row r="286" spans="1:4">
       <c r="A286" t="s">
-        <v>9447</v>
+        <v>9444</v>
       </c>
       <c r="B286" t="s">
-        <v>9448</v>
+        <v>9445</v>
       </c>
       <c r="C286" t="s">
-        <v>9397</v>
+        <v>9394</v>
       </c>
       <c r="D286" t="s">
-        <v>9398</v>
+        <v>9395</v>
       </c>
     </row>
     <row r="287" spans="1:4">
       <c r="A287" t="s">
-        <v>9449</v>
+        <v>9446</v>
       </c>
       <c r="B287" t="s">
-        <v>9450</v>
+        <v>9447</v>
       </c>
       <c r="C287" t="s">
-        <v>9397</v>
+        <v>9394</v>
       </c>
       <c r="D287" t="s">
-        <v>9398</v>
+        <v>9395</v>
       </c>
     </row>
     <row r="288" spans="1:4">
       <c r="A288" t="s">
-        <v>9451</v>
+        <v>9448</v>
       </c>
       <c r="B288" t="s">
-        <v>9452</v>
+        <v>9449</v>
       </c>
       <c r="C288" t="s">
-        <v>9397</v>
+        <v>9394</v>
       </c>
       <c r="D288" t="s">
-        <v>9398</v>
+        <v>9395</v>
       </c>
     </row>
     <row r="289" spans="1:4">
       <c r="A289" t="s">
-        <v>9453</v>
+        <v>9450</v>
       </c>
       <c r="B289" t="s">
-        <v>9454</v>
+        <v>9451</v>
       </c>
       <c r="C289" t="s">
-        <v>9397</v>
+        <v>9394</v>
       </c>
       <c r="D289" t="s">
-        <v>9398</v>
+        <v>9395</v>
       </c>
     </row>
     <row r="290" spans="1:4">
       <c r="A290" t="s">
-        <v>9455</v>
+        <v>9452</v>
       </c>
       <c r="B290" t="s">
-        <v>9456</v>
+        <v>9453</v>
       </c>
       <c r="C290" t="s">
-        <v>9397</v>
+        <v>9394</v>
       </c>
       <c r="D290" t="s">
-        <v>9398</v>
+        <v>9395</v>
       </c>
     </row>
     <row r="291" spans="1:4">
       <c r="A291" t="s">
-        <v>9457</v>
+        <v>9454</v>
       </c>
       <c r="B291" t="s">
-        <v>9458</v>
+        <v>9455</v>
       </c>
       <c r="C291" t="s">
-        <v>9397</v>
+        <v>9394</v>
       </c>
       <c r="D291" t="s">
-        <v>9398</v>
+        <v>9395</v>
       </c>
     </row>
     <row r="292" spans="1:4">
       <c r="A292" t="s">
-        <v>9459</v>
+        <v>9456</v>
       </c>
       <c r="B292" t="s">
-        <v>9460</v>
+        <v>9457</v>
       </c>
       <c r="C292" t="s">
-        <v>9397</v>
+        <v>9394</v>
       </c>
       <c r="D292" t="s">
-        <v>9398</v>
+        <v>9395</v>
       </c>
     </row>
     <row r="293" spans="1:4">
       <c r="A293" t="s">
-        <v>9461</v>
+        <v>9458</v>
       </c>
       <c r="B293" t="s">
-        <v>9462</v>
+        <v>9459</v>
       </c>
       <c r="C293" t="s">
-        <v>9397</v>
+        <v>9394</v>
       </c>
       <c r="D293" t="s">
-        <v>9398</v>
+        <v>9395</v>
       </c>
     </row>
     <row r="294" spans="1:4">
       <c r="A294" t="s">
-        <v>9463</v>
+        <v>9460</v>
       </c>
       <c r="B294" t="s">
-        <v>9464</v>
+        <v>9461</v>
       </c>
       <c r="C294" t="s">
-        <v>9397</v>
+        <v>9394</v>
       </c>
       <c r="D294" t="s">
-        <v>9398</v>
+        <v>9395</v>
       </c>
     </row>
     <row r="295" spans="1:4">
       <c r="A295" t="s">
-        <v>9465</v>
+        <v>9462</v>
       </c>
       <c r="B295" t="s">
-        <v>9466</v>
+        <v>9463</v>
       </c>
       <c r="C295" t="s">
-        <v>9397</v>
+        <v>9394</v>
       </c>
       <c r="D295" t="s">
-        <v>9398</v>
+        <v>9395</v>
       </c>
     </row>
     <row r="296" spans="1:4">
       <c r="A296" t="s">
-        <v>9467</v>
+        <v>9464</v>
       </c>
       <c r="B296" t="s">
-        <v>9468</v>
+        <v>9465</v>
       </c>
       <c r="C296" t="s">
-        <v>9397</v>
+        <v>9394</v>
       </c>
       <c r="D296" t="s">
-        <v>9398</v>
+        <v>9395</v>
       </c>
     </row>
     <row r="297" spans="1:4">
       <c r="A297" t="s">
-        <v>9469</v>
+        <v>9466</v>
       </c>
       <c r="B297" t="s">
-        <v>9470</v>
+        <v>9467</v>
       </c>
       <c r="C297" t="s">
-        <v>9397</v>
+        <v>9394</v>
       </c>
       <c r="D297" t="s">
-        <v>9398</v>
+        <v>9395</v>
       </c>
     </row>
     <row r="298" spans="1:4">
       <c r="A298" t="s">
-        <v>9471</v>
+        <v>9468</v>
       </c>
       <c r="B298" t="s">
-        <v>9472</v>
+        <v>9469</v>
       </c>
       <c r="C298" t="s">
-        <v>9397</v>
+        <v>9394</v>
       </c>
       <c r="D298" t="s">
-        <v>9398</v>
+        <v>9395</v>
       </c>
     </row>
     <row r="299" spans="1:4">
       <c r="A299" t="s">
-        <v>9473</v>
+        <v>9470</v>
       </c>
       <c r="B299" t="s">
-        <v>9474</v>
+        <v>9471</v>
       </c>
       <c r="C299" t="s">
-        <v>9397</v>
+        <v>9394</v>
       </c>
       <c r="D299" t="s">
-        <v>9398</v>
+        <v>9395</v>
       </c>
     </row>
   </sheetData>

</xml_diff>